<commit_message>
File upload with rollbacks and logs.
</commit_message>
<xml_diff>
--- a/DataUpload/ResultadoExportacion_Partidas.xlsx
+++ b/DataUpload/ResultadoExportacion_Partidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="130">
   <si>
     <t>1</t>
   </si>
@@ -414,9 +414,6 @@
   </si>
   <si>
     <t>2.16.1</t>
-  </si>
-  <si>
-    <t>99</t>
   </si>
 </sst>
 </file>
@@ -776,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="B89" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2072,7 @@
         <v>22</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>129</v>

</xml_diff>